<commit_message>
Update file template excel
</commit_message>
<xml_diff>
--- a/public/template/excel/format_laporan_operasi_2021.xlsx
+++ b/public/template/excel/format_laporan_operasi_2021.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Laphar" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1556,9 +1556,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1588,6 +1585,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2235,8 +2235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H471"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A409" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C419" sqref="C419"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2248,82 +2248,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="90"/>
-      <c r="B1" s="90"/>
+      <c r="A1" s="89"/>
+      <c r="B1" s="89"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="90"/>
-      <c r="B2" s="90"/>
+      <c r="A2" s="89"/>
+      <c r="B2" s="89"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="93"/>
-      <c r="B3" s="93"/>
+      <c r="A3" s="92"/>
+      <c r="B3" s="92"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="89" t="s">
+      <c r="A5" s="88" t="s">
         <v>280</v>
       </c>
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="91" t="s">
+      <c r="A6" s="90" t="s">
         <v>278</v>
       </c>
-      <c r="B6" s="91"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="91"/>
-      <c r="E6" s="91"/>
-      <c r="F6" s="91"/>
-      <c r="G6" s="91"/>
+      <c r="B6" s="90"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="90"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="88" t="s">
         <v>279</v>
       </c>
-      <c r="B7" s="89"/>
-      <c r="C7" s="89"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="89"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="91"/>
-      <c r="B8" s="91"/>
-      <c r="C8" s="91"/>
-      <c r="D8" s="91"/>
-      <c r="E8" s="91"/>
-      <c r="F8" s="91"/>
-      <c r="G8" s="91"/>
+      <c r="A8" s="90"/>
+      <c r="B8" s="90"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="92" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="92" t="s">
+      <c r="A9" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="94" t="s">
+      <c r="C9" s="93" t="s">
         <v>169</v>
       </c>
-      <c r="D9" s="95"/>
-      <c r="E9" s="96" t="s">
+      <c r="D9" s="94"/>
+      <c r="E9" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="97"/>
-      <c r="G9" s="92" t="s">
+      <c r="F9" s="96"/>
+      <c r="G9" s="91" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="92"/>
-      <c r="B10" s="92"/>
+      <c r="A10" s="91"/>
+      <c r="B10" s="91"/>
       <c r="C10" s="24">
         <v>2019</v>
       </c>
@@ -2336,7 +2336,7 @@
       <c r="F10" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="92"/>
+      <c r="G10" s="91"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -2447,9 +2447,11 @@
         <v>11</v>
       </c>
       <c r="C16" s="27">
+        <f>SUM(C14:C15)</f>
         <v>0</v>
       </c>
       <c r="D16" s="27">
+        <f>SUM(D14:D15)</f>
         <v>0</v>
       </c>
       <c r="E16" s="49" t="str">
@@ -2907,9 +2909,11 @@
         <v>31</v>
       </c>
       <c r="C36" s="27">
+        <f>SUM(C19:C35)</f>
         <v>0</v>
       </c>
       <c r="D36" s="27">
+        <f>SUM(D19:D35)</f>
         <v>0</v>
       </c>
       <c r="E36" s="49" t="str">
@@ -3346,9 +3350,11 @@
         <v>202</v>
       </c>
       <c r="C55" s="27">
+        <f>SUM(C38:C54)</f>
         <v>0</v>
       </c>
       <c r="D55" s="27">
+        <f>SUM(D38:D54)</f>
         <v>0</v>
       </c>
       <c r="E55" s="49" t="str">
@@ -3508,9 +3514,11 @@
         <v>174</v>
       </c>
       <c r="C63" s="27">
+        <f>SUM(C60:C62)</f>
         <v>0</v>
       </c>
       <c r="D63" s="27">
+        <f>SUM(D60:D62)</f>
         <v>0</v>
       </c>
       <c r="E63" s="49" t="str">
@@ -3671,9 +3679,11 @@
         <v>205</v>
       </c>
       <c r="C70" s="27">
+        <f>SUM(C65:C69)</f>
         <v>0</v>
       </c>
       <c r="D70" s="27">
+        <f>SUM(D65:D69)</f>
         <v>0</v>
       </c>
       <c r="E70" s="49" t="str">
@@ -3884,9 +3894,11 @@
         <v>206</v>
       </c>
       <c r="C79" s="27">
+        <f>SUM(C72:C78)</f>
         <v>0</v>
       </c>
       <c r="D79" s="27">
+        <f>SUM(D72:D78)</f>
         <v>0</v>
       </c>
       <c r="E79" s="49" t="str">
@@ -4185,9 +4197,11 @@
         <v>206</v>
       </c>
       <c r="C92" s="27">
+        <f>SUM(C81:C91)</f>
         <v>0</v>
       </c>
       <c r="D92" s="27">
+        <f>SUM(D81:D91)</f>
         <v>0</v>
       </c>
       <c r="E92" s="49" t="str">
@@ -4471,9 +4485,11 @@
         <v>207</v>
       </c>
       <c r="C104" s="27">
+        <f>SUM(C94:C103)</f>
         <v>0</v>
       </c>
       <c r="D104" s="27">
+        <f>SUM(D94:D103)</f>
         <v>0</v>
       </c>
       <c r="E104" s="49" t="str">
@@ -11385,9 +11401,9 @@
       <c r="B415" s="46"/>
       <c r="C415" s="46"/>
       <c r="D415" s="46"/>
-      <c r="E415" s="88"/>
-      <c r="F415" s="88"/>
-      <c r="G415" s="88"/>
+      <c r="E415" s="87"/>
+      <c r="F415" s="87"/>
+      <c r="G415" s="87"/>
     </row>
     <row r="416" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A416" s="46"/>
@@ -11403,10 +11419,10 @@
       <c r="B417" s="46"/>
       <c r="C417" s="46"/>
       <c r="D417" s="46"/>
-      <c r="E417" s="87" t="s">
+      <c r="E417" s="97" t="s">
         <v>293</v>
       </c>
-      <c r="F417" s="87"/>
+      <c r="F417" s="97"/>
       <c r="G417" s="46"/>
     </row>
     <row r="418" spans="1:7" x14ac:dyDescent="0.25">
@@ -11414,8 +11430,8 @@
       <c r="B418" s="46"/>
       <c r="C418" s="46"/>
       <c r="D418" s="46"/>
-      <c r="E418" s="87"/>
-      <c r="F418" s="87"/>
+      <c r="E418" s="97"/>
+      <c r="F418" s="97"/>
       <c r="G418" s="46"/>
     </row>
     <row r="419" spans="1:7" x14ac:dyDescent="0.25">
@@ -11423,10 +11439,10 @@
       <c r="B419" s="46"/>
       <c r="C419" s="86"/>
       <c r="D419" s="46"/>
-      <c r="E419" s="88" t="s">
+      <c r="E419" s="87" t="s">
         <v>294</v>
       </c>
-      <c r="F419" s="88"/>
+      <c r="F419" s="87"/>
       <c r="G419" s="46"/>
     </row>
     <row r="420" spans="1:7" x14ac:dyDescent="0.25">
@@ -11470,10 +11486,10 @@
       <c r="B424" s="46"/>
       <c r="C424" s="86"/>
       <c r="D424" s="46"/>
-      <c r="E424" s="87" t="s">
+      <c r="E424" s="97" t="s">
         <v>295</v>
       </c>
-      <c r="F424" s="87"/>
+      <c r="F424" s="97"/>
       <c r="G424" s="46"/>
     </row>
     <row r="425" spans="1:7" x14ac:dyDescent="0.25">
@@ -11481,10 +11497,10 @@
       <c r="B425" s="46"/>
       <c r="C425" s="86"/>
       <c r="D425" s="46"/>
-      <c r="E425" s="87" t="s">
+      <c r="E425" s="97" t="s">
         <v>296</v>
       </c>
-      <c r="F425" s="87"/>
+      <c r="F425" s="97"/>
       <c r="G425" s="46"/>
     </row>
     <row r="426" spans="1:7" x14ac:dyDescent="0.25">
@@ -11867,6 +11883,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="E418:F418"/>
+    <mergeCell ref="E419:F419"/>
+    <mergeCell ref="E424:F424"/>
+    <mergeCell ref="E425:F425"/>
+    <mergeCell ref="E417:F417"/>
     <mergeCell ref="E415:G415"/>
     <mergeCell ref="A7:G7"/>
     <mergeCell ref="A1:B1"/>
@@ -11880,11 +11901,6 @@
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E418:F418"/>
-    <mergeCell ref="E419:F419"/>
-    <mergeCell ref="E424:F424"/>
-    <mergeCell ref="E425:F425"/>
-    <mergeCell ref="E417:F417"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.31496062992125984" top="0.23622047244094491" bottom="0.23622047244094491" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Update format report excel
</commit_message>
<xml_diff>
--- a/public/template/excel/format_laporan_operasi_2021.xlsx
+++ b/public/template/excel/format_laporan_operasi_2021.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\korlantas\public\template\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u117nxs\Desktop\blog post\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A373E48-FA0D-4AC3-A68B-FADBCBDA24E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2664" windowWidth="25596" windowHeight="15996"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Laphar" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -22,7 +23,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -998,9 +998,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -1350,7 +1350,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1409,7 +1409,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1477,7 +1477,7 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="11" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1542,9 +1542,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1556,6 +1553,9 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1586,13 +1586,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1800,149 +1797,6 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>129</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>795411</xdr:colOff>
-      <xdr:row>131</xdr:row>
-      <xdr:rowOff>39132</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="TextBox 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EF909F5-AB16-394B-84E9-EC17F477A9D1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="317500" y="21297900"/>
-          <a:ext cx="795411" cy="369332"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="en-US"/>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t>Sumut</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2022,6 +1876,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2057,6 +1928,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2232,34 +2120,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H471"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="110" zoomScaleSheetLayoutView="110" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D417" sqref="D417"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="53.44140625" style="2" customWidth="1"/>
-    <col min="3" max="7" width="12.77734375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="4.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="53.42578125" style="2" customWidth="1"/>
+    <col min="3" max="7" width="12.7109375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="89"/>
       <c r="B1" s="89"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="89"/>
       <c r="B2" s="89"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="92"/>
       <c r="B3" s="92"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="88" t="s">
         <v>280</v>
       </c>
@@ -2270,7 +2158,7 @@
       <c r="F5" s="88"/>
       <c r="G5" s="88"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="90" t="s">
         <v>278</v>
       </c>
@@ -2281,7 +2169,7 @@
       <c r="F6" s="90"/>
       <c r="G6" s="90"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="88" t="s">
         <v>279</v>
       </c>
@@ -2293,7 +2181,7 @@
       <c r="G7" s="88"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="90"/>
       <c r="B8" s="90"/>
       <c r="C8" s="90"/>
@@ -2302,7 +2190,7 @@
       <c r="F8" s="90"/>
       <c r="G8" s="90"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="91" t="s">
         <v>0</v>
       </c>
@@ -2321,7 +2209,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="91"/>
       <c r="B10" s="91"/>
       <c r="C10" s="24">
@@ -2338,7 +2226,7 @@
       </c>
       <c r="G10" s="91"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -2361,7 +2249,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>230</v>
       </c>
@@ -2374,7 +2262,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>1</v>
       </c>
@@ -2389,7 +2277,7 @@
       </c>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>8</v>
       </c>
@@ -2414,7 +2302,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
@@ -2439,7 +2327,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
@@ -2466,7 +2354,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>2</v>
       </c>
@@ -2481,7 +2369,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>8</v>
       </c>
@@ -2496,7 +2384,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>8</v>
       </c>
@@ -2521,7 +2409,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>8</v>
       </c>
@@ -2546,7 +2434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
       <c r="B21" s="5" t="s">
         <v>16</v>
@@ -2569,7 +2457,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>8</v>
       </c>
@@ -2594,7 +2482,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>8</v>
       </c>
@@ -2619,7 +2507,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>8</v>
       </c>
@@ -2644,7 +2532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
       <c r="B25" s="5" t="s">
         <v>20</v>
@@ -2667,7 +2555,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="s">
         <v>21</v>
@@ -2690,7 +2578,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
       <c r="B27" s="5" t="s">
         <v>22</v>
@@ -2713,7 +2601,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
       <c r="B28" s="5" t="s">
         <v>23</v>
@@ -2736,7 +2624,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
       <c r="B29" s="5" t="s">
         <v>24</v>
@@ -2759,7 +2647,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
       <c r="B30" s="5" t="s">
         <v>25</v>
@@ -2782,7 +2670,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="5"/>
       <c r="B31" s="5" t="s">
         <v>26</v>
@@ -2805,7 +2693,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
       <c r="B32" s="5" t="s">
         <v>27</v>
@@ -2828,7 +2716,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
       <c r="B33" s="5" t="s">
         <v>28</v>
@@ -2851,7 +2739,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>8</v>
       </c>
@@ -2876,7 +2764,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>8</v>
       </c>
@@ -2901,7 +2789,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>8</v>
       </c>
@@ -2928,7 +2816,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>8</v>
       </c>
@@ -2941,9 +2829,9 @@
       <c r="F37" s="50"/>
       <c r="G37" s="30"/>
     </row>
-    <row r="38" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="84"/>
-      <c r="B38" s="85" t="s">
+    <row r="38" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="83"/>
+      <c r="B38" s="84" t="s">
         <v>33</v>
       </c>
       <c r="C38" s="67">
@@ -2964,9 +2852,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="84"/>
-      <c r="B39" s="85" t="s">
+    <row r="39" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="83"/>
+      <c r="B39" s="84" t="s">
         <v>34</v>
       </c>
       <c r="C39" s="67">
@@ -2987,9 +2875,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="84"/>
-      <c r="B40" s="85" t="s">
+    <row r="40" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="83"/>
+      <c r="B40" s="84" t="s">
         <v>35</v>
       </c>
       <c r="C40" s="67">
@@ -3010,9 +2898,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="84"/>
-      <c r="B41" s="85" t="s">
+    <row r="41" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="83"/>
+      <c r="B41" s="84" t="s">
         <v>17</v>
       </c>
       <c r="C41" s="67">
@@ -3033,9 +2921,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="84"/>
-      <c r="B42" s="85" t="s">
+    <row r="42" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="83"/>
+      <c r="B42" s="84" t="s">
         <v>36</v>
       </c>
       <c r="C42" s="67">
@@ -3056,9 +2944,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="84"/>
-      <c r="B43" s="85" t="s">
+    <row r="43" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="83"/>
+      <c r="B43" s="84" t="s">
         <v>37</v>
       </c>
       <c r="C43" s="67">
@@ -3079,9 +2967,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="84"/>
-      <c r="B44" s="85" t="s">
+    <row r="44" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="83"/>
+      <c r="B44" s="84" t="s">
         <v>20</v>
       </c>
       <c r="C44" s="67">
@@ -3102,9 +2990,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="84"/>
-      <c r="B45" s="85" t="s">
+    <row r="45" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="83"/>
+      <c r="B45" s="84" t="s">
         <v>21</v>
       </c>
       <c r="C45" s="67">
@@ -3125,9 +3013,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="84"/>
-      <c r="B46" s="85" t="s">
+    <row r="46" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="83"/>
+      <c r="B46" s="84" t="s">
         <v>38</v>
       </c>
       <c r="C46" s="67">
@@ -3148,9 +3036,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="84"/>
-      <c r="B47" s="85" t="s">
+    <row r="47" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="83"/>
+      <c r="B47" s="84" t="s">
         <v>39</v>
       </c>
       <c r="C47" s="67">
@@ -3171,9 +3059,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="84"/>
-      <c r="B48" s="85" t="s">
+    <row r="48" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="83"/>
+      <c r="B48" s="84" t="s">
         <v>24</v>
       </c>
       <c r="C48" s="67">
@@ -3194,11 +3082,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="85" t="s">
-        <v>8</v>
-      </c>
-      <c r="B49" s="85" t="s">
+    <row r="49" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="84" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" s="84" t="s">
         <v>25</v>
       </c>
       <c r="C49" s="67">
@@ -3219,11 +3107,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="85" t="s">
-        <v>8</v>
-      </c>
-      <c r="B50" s="85" t="s">
+    <row r="50" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="84" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="84" t="s">
         <v>26</v>
       </c>
       <c r="C50" s="67">
@@ -3244,11 +3132,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="85" t="s">
-        <v>8</v>
-      </c>
-      <c r="B51" s="85" t="s">
+    <row r="51" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="84" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" s="84" t="s">
         <v>27</v>
       </c>
       <c r="C51" s="67">
@@ -3269,11 +3157,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="85" t="s">
-        <v>8</v>
-      </c>
-      <c r="B52" s="85" t="s">
+    <row r="52" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="84" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" s="84" t="s">
         <v>28</v>
       </c>
       <c r="C52" s="67">
@@ -3294,11 +3182,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="85" t="s">
-        <v>8</v>
-      </c>
-      <c r="B53" s="85" t="s">
+    <row r="53" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="84" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" s="84" t="s">
         <v>29</v>
       </c>
       <c r="C53" s="67">
@@ -3319,9 +3207,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="85"/>
-      <c r="B54" s="85" t="s">
+    <row r="54" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="84"/>
+      <c r="B54" s="84" t="s">
         <v>30</v>
       </c>
       <c r="C54" s="67">
@@ -3342,7 +3230,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>8</v>
       </c>
@@ -3369,7 +3257,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
       <c r="B56" s="4" t="s">
         <v>40</v>
@@ -3380,7 +3268,7 @@
       <c r="F56" s="50"/>
       <c r="G56" s="30"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
       <c r="B57" s="5" t="s">
         <v>41</v>
@@ -3402,7 +3290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>8</v>
       </c>
@@ -3426,7 +3314,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="8">
         <v>3</v>
       </c>
@@ -3439,7 +3327,7 @@
       <c r="F59" s="50"/>
       <c r="G59" s="29"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="10"/>
       <c r="B60" s="11" t="s">
         <v>171</v>
@@ -3462,7 +3350,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="10"/>
       <c r="B61" s="11" t="s">
         <v>172</v>
@@ -3485,7 +3373,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="10"/>
       <c r="B62" s="11" t="s">
         <v>173</v>
@@ -3508,7 +3396,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="10"/>
       <c r="B63" s="9" t="s">
         <v>174</v>
@@ -3533,7 +3421,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>4</v>
       </c>
@@ -3546,7 +3434,7 @@
       <c r="F64" s="50"/>
       <c r="G64" s="30"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>8</v>
       </c>
@@ -3571,7 +3459,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
         <v>8</v>
       </c>
@@ -3596,7 +3484,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>8</v>
       </c>
@@ -3621,7 +3509,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="12" t="s">
         <v>8</v>
       </c>
@@ -3646,7 +3534,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>8</v>
       </c>
@@ -3671,7 +3559,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>8</v>
       </c>
@@ -3698,7 +3586,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <v>5</v>
       </c>
@@ -3711,7 +3599,7 @@
       <c r="F71" s="50"/>
       <c r="G71" s="30"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
         <v>8</v>
       </c>
@@ -3736,7 +3624,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
         <v>8</v>
       </c>
@@ -3761,7 +3649,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
         <v>8</v>
       </c>
@@ -3786,7 +3674,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>8</v>
       </c>
@@ -3811,7 +3699,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>8</v>
       </c>
@@ -3836,7 +3724,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
         <v>8</v>
       </c>
@@ -3861,7 +3749,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
         <v>8</v>
       </c>
@@ -3886,7 +3774,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>8</v>
       </c>
@@ -3913,7 +3801,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
         <v>6</v>
       </c>
@@ -3926,7 +3814,7 @@
       <c r="F80" s="50"/>
       <c r="G80" s="30"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="4"/>
       <c r="B81" s="5" t="s">
         <v>57</v>
@@ -3949,7 +3837,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
         <v>8</v>
       </c>
@@ -3974,7 +3862,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
         <v>8</v>
       </c>
@@ -3999,7 +3887,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
         <v>8</v>
       </c>
@@ -4024,7 +3912,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
         <v>8</v>
       </c>
@@ -4049,7 +3937,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="5"/>
       <c r="B86" s="5" t="s">
         <v>63</v>
@@ -4072,7 +3960,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="5"/>
       <c r="B87" s="5" t="s">
         <v>64</v>
@@ -4095,7 +3983,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="5"/>
       <c r="B88" s="5" t="s">
         <v>65</v>
@@ -4118,7 +4006,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
         <v>8</v>
       </c>
@@ -4143,7 +4031,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="5"/>
       <c r="B90" s="5" t="s">
         <v>67</v>
@@ -4166,7 +4054,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="5"/>
       <c r="B91" s="5" t="s">
         <v>68</v>
@@ -4189,7 +4077,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>8</v>
       </c>
@@ -4216,7 +4104,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="4">
         <v>7</v>
       </c>
@@ -4229,7 +4117,7 @@
       <c r="F93" s="50"/>
       <c r="G93" s="30"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
         <v>8</v>
       </c>
@@ -4254,7 +4142,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
         <v>8</v>
       </c>
@@ -4279,7 +4167,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
         <v>8</v>
       </c>
@@ -4304,7 +4192,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
         <v>8</v>
       </c>
@@ -4329,7 +4217,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
         <v>8</v>
       </c>
@@ -4354,7 +4242,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
         <v>8</v>
       </c>
@@ -4379,7 +4267,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="5"/>
       <c r="B100" s="5" t="s">
         <v>77</v>
@@ -4402,7 +4290,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
         <v>8</v>
       </c>
@@ -4427,7 +4315,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
         <v>8</v>
       </c>
@@ -4452,7 +4340,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
         <v>8</v>
       </c>
@@ -4477,7 +4365,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>8</v>
       </c>
@@ -4504,7 +4392,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="4">
         <v>8</v>
       </c>
@@ -4517,7 +4405,7 @@
       <c r="F105" s="50"/>
       <c r="G105" s="30"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="4"/>
       <c r="B106" s="4" t="s">
         <v>121</v>
@@ -4528,7 +4416,7 @@
       <c r="F106" s="50"/>
       <c r="G106" s="30"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="4"/>
       <c r="B107" s="5" t="s">
         <v>122</v>
@@ -4551,7 +4439,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="4"/>
       <c r="B108" s="5" t="s">
         <v>123</v>
@@ -4574,7 +4462,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="4"/>
       <c r="B109" s="5" t="s">
         <v>124</v>
@@ -4597,7 +4485,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="4"/>
       <c r="B110" s="5" t="s">
         <v>125</v>
@@ -4620,7 +4508,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="4"/>
       <c r="B111" s="5" t="s">
         <v>126</v>
@@ -4643,15 +4531,17 @@
         <v>83</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="4"/>
       <c r="B112" s="4" t="s">
         <v>208</v>
       </c>
       <c r="C112" s="27">
+        <f>SUM(C107:C111)</f>
         <v>0</v>
       </c>
       <c r="D112" s="27">
+        <f>SUM(D107:D111)</f>
         <v>0</v>
       </c>
       <c r="E112" s="49" t="str">
@@ -4666,7 +4556,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" s="4"/>
       <c r="B113" s="4" t="s">
         <v>127</v>
@@ -4677,7 +4567,7 @@
       <c r="F113" s="50"/>
       <c r="G113" s="30"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" s="4"/>
       <c r="B114" s="5" t="s">
         <v>82</v>
@@ -4700,7 +4590,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="4"/>
       <c r="B115" s="5" t="s">
         <v>84</v>
@@ -4723,7 +4613,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" s="4"/>
       <c r="B116" s="5" t="s">
         <v>85</v>
@@ -4746,7 +4636,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" s="4"/>
       <c r="B117" s="5" t="s">
         <v>86</v>
@@ -4769,15 +4659,17 @@
         <v>83</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" s="4"/>
       <c r="B118" s="4" t="s">
         <v>206</v>
       </c>
       <c r="C118" s="27">
+        <f>SUM(C114:C117)</f>
         <v>0</v>
       </c>
       <c r="D118" s="27">
+        <f>SUM(D114:D117)</f>
         <v>0</v>
       </c>
       <c r="E118" s="49" t="str">
@@ -4792,7 +4684,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" s="4"/>
       <c r="B119" s="4" t="s">
         <v>128</v>
@@ -4803,7 +4695,7 @@
       <c r="F119" s="50"/>
       <c r="G119" s="30"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" s="4"/>
       <c r="B120" s="5" t="s">
         <v>87</v>
@@ -4826,7 +4718,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" s="4"/>
       <c r="B121" s="5" t="s">
         <v>88</v>
@@ -4849,7 +4741,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" s="4"/>
       <c r="B122" s="5" t="s">
         <v>89</v>
@@ -4872,7 +4764,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" s="4"/>
       <c r="B123" s="5" t="s">
         <v>90</v>
@@ -4895,15 +4787,17 @@
         <v>83</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" s="4"/>
       <c r="B124" s="4" t="s">
         <v>204</v>
       </c>
       <c r="C124" s="27">
+        <f>SUM(C120:C123)</f>
         <v>0</v>
       </c>
       <c r="D124" s="27">
+        <f>SUM(D120:D123)</f>
         <v>0</v>
       </c>
       <c r="E124" s="49" t="str">
@@ -4918,7 +4812,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" s="13" t="s">
         <v>231</v>
       </c>
@@ -4931,7 +4825,7 @@
       <c r="F125" s="50"/>
       <c r="G125" s="30"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" s="4">
         <v>9</v>
       </c>
@@ -4944,7 +4838,7 @@
       <c r="F126" s="50"/>
       <c r="G126" s="30"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" s="5" t="s">
         <v>8</v>
       </c>
@@ -4969,7 +4863,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" s="5" t="s">
         <v>8</v>
       </c>
@@ -4994,7 +4888,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" s="5" t="s">
         <v>8</v>
       </c>
@@ -5019,7 +4913,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" s="5" t="s">
         <v>8</v>
       </c>
@@ -5044,7 +4938,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" s="5" t="s">
         <v>8</v>
       </c>
@@ -5069,7 +4963,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" s="4">
         <v>10</v>
       </c>
@@ -5082,7 +4976,7 @@
       <c r="F132" s="50"/>
       <c r="G132" s="29"/>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" s="5"/>
       <c r="B133" s="11" t="s">
         <v>171</v>
@@ -5105,7 +4999,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" s="5"/>
       <c r="B134" s="11" t="s">
         <v>172</v>
@@ -5128,7 +5022,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" s="5"/>
       <c r="B135" s="11" t="s">
         <v>173</v>
@@ -5151,15 +5045,17 @@
         <v>44</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" s="5"/>
       <c r="B136" s="9" t="s">
         <v>174</v>
       </c>
       <c r="C136" s="27">
+        <f>SUM(C133:C135)</f>
         <v>0</v>
       </c>
       <c r="D136" s="27">
+        <f>SUM(D133:D135)</f>
         <v>0</v>
       </c>
       <c r="E136" s="49" t="str">
@@ -5174,7 +5070,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" s="4">
         <v>11</v>
       </c>
@@ -5187,7 +5083,7 @@
       <c r="F137" s="50"/>
       <c r="G137" s="33"/>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" s="5" t="s">
         <v>8</v>
       </c>
@@ -5212,7 +5108,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" s="5" t="s">
         <v>8</v>
       </c>
@@ -5237,7 +5133,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" s="12" t="s">
         <v>8</v>
       </c>
@@ -5262,7 +5158,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" s="5" t="s">
         <v>8</v>
       </c>
@@ -5287,7 +5183,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" s="5" t="s">
         <v>8</v>
       </c>
@@ -5312,7 +5208,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" s="5" t="s">
         <v>8</v>
       </c>
@@ -5337,7 +5233,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" s="5" t="s">
         <v>8</v>
       </c>
@@ -5362,7 +5258,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
         <v>8</v>
       </c>
@@ -5370,9 +5266,11 @@
         <v>209</v>
       </c>
       <c r="C145" s="27">
+        <f>SUM(C138:C144)</f>
         <v>0</v>
       </c>
       <c r="D145" s="27">
+        <f>SUM(D138:D144)</f>
         <v>0</v>
       </c>
       <c r="E145" s="49" t="str">
@@ -5387,7 +5285,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" s="4">
         <v>12</v>
       </c>
@@ -5400,7 +5298,7 @@
       <c r="F146" s="50"/>
       <c r="G146" s="33"/>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" s="4"/>
       <c r="B147" s="5" t="s">
         <v>57</v>
@@ -5423,7 +5321,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" s="4"/>
       <c r="B148" s="5" t="s">
         <v>59</v>
@@ -5446,7 +5344,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" s="4"/>
       <c r="B149" s="5" t="s">
         <v>60</v>
@@ -5469,7 +5367,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" s="4"/>
       <c r="B150" s="5" t="s">
         <v>61</v>
@@ -5492,7 +5390,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" s="4"/>
       <c r="B151" s="5" t="s">
         <v>62</v>
@@ -5515,7 +5413,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" s="4"/>
       <c r="B152" s="5" t="s">
         <v>63</v>
@@ -5538,7 +5436,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" s="5" t="s">
         <v>8</v>
       </c>
@@ -5563,7 +5461,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" s="5" t="s">
         <v>8</v>
       </c>
@@ -5588,7 +5486,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" s="5" t="s">
         <v>8</v>
       </c>
@@ -5613,7 +5511,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" s="5" t="s">
         <v>8</v>
       </c>
@@ -5638,7 +5536,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" s="14" t="s">
         <v>8</v>
       </c>
@@ -5663,7 +5561,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" s="15" t="s">
         <v>8</v>
       </c>
@@ -5671,9 +5569,11 @@
         <v>210</v>
       </c>
       <c r="C158" s="27">
+        <f>SUM(C147:C157)</f>
         <v>0</v>
       </c>
       <c r="D158" s="27">
+        <f>SUM(D147:D157)</f>
         <v>0</v>
       </c>
       <c r="E158" s="49" t="str">
@@ -5688,7 +5588,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" s="4">
         <v>13</v>
       </c>
@@ -5701,7 +5601,7 @@
       <c r="F159" s="50"/>
       <c r="G159" s="37"/>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" s="5" t="s">
         <v>8</v>
       </c>
@@ -5726,7 +5626,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" s="5" t="s">
         <v>8</v>
       </c>
@@ -5751,7 +5651,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" s="5" t="s">
         <v>8</v>
       </c>
@@ -5776,7 +5676,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" s="5" t="s">
         <v>8</v>
       </c>
@@ -5801,7 +5701,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" s="5" t="s">
         <v>8</v>
       </c>
@@ -5826,7 +5726,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" s="5" t="s">
         <v>8</v>
       </c>
@@ -5851,7 +5751,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" s="5"/>
       <c r="B166" s="5" t="s">
         <v>77</v>
@@ -5874,7 +5774,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" s="5" t="s">
         <v>8</v>
       </c>
@@ -5899,7 +5799,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" s="5"/>
       <c r="B168" s="17" t="s">
         <v>79</v>
@@ -5922,7 +5822,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" s="5" t="s">
         <v>8</v>
       </c>
@@ -5947,7 +5847,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" s="4" t="s">
         <v>8</v>
       </c>
@@ -5955,9 +5855,11 @@
         <v>209</v>
       </c>
       <c r="C170" s="27">
+        <f>SUM(C160:C169)</f>
         <v>0</v>
       </c>
       <c r="D170" s="27">
+        <f>SUM(D160:D169)</f>
         <v>0</v>
       </c>
       <c r="E170" s="49" t="str">
@@ -5972,7 +5874,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" s="4">
         <v>14</v>
       </c>
@@ -5985,7 +5887,7 @@
       <c r="F171" s="50"/>
       <c r="G171" s="30"/>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" s="5" t="s">
         <v>8</v>
       </c>
@@ -6010,7 +5912,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" s="5" t="s">
         <v>8</v>
       </c>
@@ -6035,7 +5937,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" s="5" t="s">
         <v>8</v>
       </c>
@@ -6060,7 +5962,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" s="5" t="s">
         <v>8</v>
       </c>
@@ -6085,7 +5987,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" s="5" t="s">
         <v>8</v>
       </c>
@@ -6110,7 +6012,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" s="5" t="s">
         <v>8</v>
       </c>
@@ -6135,7 +6037,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" s="4" t="s">
         <v>8</v>
       </c>
@@ -6143,9 +6045,11 @@
         <v>270</v>
       </c>
       <c r="C178" s="27">
+        <f>SUM(C172:C177)</f>
         <v>0</v>
       </c>
       <c r="D178" s="27">
+        <f>SUM(D172:D177)</f>
         <v>0</v>
       </c>
       <c r="E178" s="49" t="str">
@@ -6160,7 +6064,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" s="4">
         <v>15</v>
       </c>
@@ -6173,7 +6077,7 @@
       <c r="F179" s="50"/>
       <c r="G179" s="30"/>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" s="5" t="s">
         <v>8</v>
       </c>
@@ -6198,7 +6102,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" s="5" t="s">
         <v>8</v>
       </c>
@@ -6223,7 +6127,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" s="5" t="s">
         <v>8</v>
       </c>
@@ -6248,7 +6152,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" s="5"/>
       <c r="B183" s="5" t="s">
         <v>110</v>
@@ -6271,7 +6175,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" s="5" t="s">
         <v>8</v>
       </c>
@@ -6296,7 +6200,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" s="5" t="s">
         <v>8</v>
       </c>
@@ -6321,7 +6225,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" s="5" t="s">
         <v>8</v>
       </c>
@@ -6346,7 +6250,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" s="6" t="s">
         <v>8</v>
       </c>
@@ -6371,7 +6275,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" s="5"/>
       <c r="B188" s="5" t="s">
         <v>115</v>
@@ -6394,7 +6298,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" s="5" t="s">
         <v>8</v>
       </c>
@@ -6419,7 +6323,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" s="4" t="s">
         <v>8</v>
       </c>
@@ -6427,9 +6331,11 @@
         <v>211</v>
       </c>
       <c r="C190" s="27">
+        <f>SUM(C180:C189)</f>
         <v>0</v>
       </c>
       <c r="D190" s="27">
+        <f>SUM(D180:D189)</f>
         <v>0</v>
       </c>
       <c r="E190" s="49" t="str">
@@ -6444,7 +6350,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191" s="4">
         <v>16</v>
       </c>
@@ -6457,7 +6363,7 @@
       <c r="F191" s="50"/>
       <c r="G191" s="30"/>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192" s="5" t="s">
         <v>8</v>
       </c>
@@ -6482,7 +6388,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193" s="5" t="s">
         <v>8</v>
       </c>
@@ -6507,7 +6413,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A194" s="5" t="s">
         <v>8</v>
       </c>
@@ -6532,7 +6438,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A195" s="5" t="s">
         <v>8</v>
       </c>
@@ -6557,7 +6463,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A196" s="5" t="s">
         <v>8</v>
       </c>
@@ -6582,7 +6488,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A197" s="5" t="s">
         <v>8</v>
       </c>
@@ -6607,7 +6513,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A198" s="5" t="s">
         <v>8</v>
       </c>
@@ -6632,7 +6538,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A199" s="4" t="s">
         <v>8</v>
       </c>
@@ -6640,9 +6546,11 @@
         <v>212</v>
       </c>
       <c r="C199" s="27">
+        <f>SUM(C192:C198)</f>
         <v>0</v>
       </c>
       <c r="D199" s="27">
+        <f>SUM(D192:D198)</f>
         <v>0</v>
       </c>
       <c r="E199" s="49" t="str">
@@ -6657,7 +6565,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A200" s="4">
         <v>17</v>
       </c>
@@ -6670,7 +6578,7 @@
       <c r="F200" s="50"/>
       <c r="G200" s="30"/>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201" s="4"/>
       <c r="B201" s="5" t="s">
         <v>57</v>
@@ -6693,7 +6601,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A202" s="4"/>
       <c r="B202" s="5" t="s">
         <v>59</v>
@@ -6716,7 +6624,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203" s="4"/>
       <c r="B203" s="5" t="s">
         <v>60</v>
@@ -6739,7 +6647,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A204" s="4"/>
       <c r="B204" s="5" t="s">
         <v>61</v>
@@ -6762,7 +6670,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A205" s="4"/>
       <c r="B205" s="5" t="s">
         <v>62</v>
@@ -6785,7 +6693,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206" s="4"/>
       <c r="B206" s="5" t="s">
         <v>63</v>
@@ -6808,7 +6716,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A207" s="4"/>
       <c r="B207" s="5" t="s">
         <v>64</v>
@@ -6831,7 +6739,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A208" s="5" t="s">
         <v>8</v>
       </c>
@@ -6856,7 +6764,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A209" s="5" t="s">
         <v>8</v>
       </c>
@@ -6881,7 +6789,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A210" s="5" t="s">
         <v>8</v>
       </c>
@@ -6906,7 +6814,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A211" s="5" t="s">
         <v>8</v>
       </c>
@@ -6931,7 +6839,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A212" s="4" t="s">
         <v>8</v>
       </c>
@@ -6939,9 +6847,11 @@
         <v>213</v>
       </c>
       <c r="C212" s="27">
+        <f>SUM(C201:C211)</f>
         <v>0</v>
       </c>
       <c r="D212" s="27">
+        <f>SUM(D201:D211)</f>
         <v>0</v>
       </c>
       <c r="E212" s="49" t="str">
@@ -6956,7 +6866,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A213" s="18">
         <v>18</v>
       </c>
@@ -6969,7 +6879,7 @@
       <c r="F213" s="50"/>
       <c r="G213" s="39"/>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A214" s="5" t="s">
         <v>8</v>
       </c>
@@ -6994,7 +6904,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A215" s="5" t="s">
         <v>8</v>
       </c>
@@ -7019,7 +6929,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A216" s="5" t="s">
         <v>8</v>
       </c>
@@ -7044,7 +6954,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A217" s="5" t="s">
         <v>8</v>
       </c>
@@ -7069,7 +6979,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A218" s="5" t="s">
         <v>8</v>
       </c>
@@ -7094,7 +7004,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A219" s="5" t="s">
         <v>8</v>
       </c>
@@ -7119,7 +7029,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A220" s="5"/>
       <c r="B220" s="5" t="s">
         <v>77</v>
@@ -7142,7 +7052,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A221" s="5"/>
       <c r="B221" s="5" t="s">
         <v>78</v>
@@ -7165,7 +7075,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A222" s="5" t="s">
         <v>8</v>
       </c>
@@ -7190,7 +7100,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A223" s="5" t="s">
         <v>8</v>
       </c>
@@ -7215,7 +7125,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A224" s="4" t="s">
         <v>8</v>
       </c>
@@ -7223,9 +7133,11 @@
         <v>214</v>
       </c>
       <c r="C224" s="27">
+        <f>SUM(C214:C223)</f>
         <v>0</v>
       </c>
       <c r="D224" s="27">
+        <f>SUM(D214:D223)</f>
         <v>0</v>
       </c>
       <c r="E224" s="49" t="str">
@@ -7240,7 +7152,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A225" s="4">
         <v>19</v>
       </c>
@@ -7253,7 +7165,7 @@
       <c r="F225" s="50"/>
       <c r="G225" s="30"/>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A226" s="5" t="s">
         <v>8</v>
       </c>
@@ -7266,7 +7178,7 @@
       <c r="F226" s="50"/>
       <c r="G226" s="29"/>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A227" s="5" t="s">
         <v>8</v>
       </c>
@@ -7291,7 +7203,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A228" s="5" t="s">
         <v>8</v>
       </c>
@@ -7316,7 +7228,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A229" s="5" t="s">
         <v>8</v>
       </c>
@@ -7341,7 +7253,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A230" s="5" t="s">
         <v>8</v>
       </c>
@@ -7366,7 +7278,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A231" s="5"/>
       <c r="B231" s="5" t="s">
         <v>126</v>
@@ -7389,7 +7301,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A232" s="5" t="s">
         <v>8</v>
       </c>
@@ -7414,7 +7326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A233" s="4" t="s">
         <v>8</v>
       </c>
@@ -7422,9 +7334,11 @@
         <v>215</v>
       </c>
       <c r="C233" s="27">
+        <f>SUM(C227:C232)</f>
         <v>0</v>
       </c>
       <c r="D233" s="27">
+        <f>SUM(D227:D232)</f>
         <v>0</v>
       </c>
       <c r="E233" s="49" t="str">
@@ -7439,7 +7353,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A234" s="4" t="s">
         <v>8</v>
       </c>
@@ -7452,7 +7366,7 @@
       <c r="F234" s="50"/>
       <c r="G234" s="30"/>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A235" s="5" t="s">
         <v>8</v>
       </c>
@@ -7477,7 +7391,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A236" s="5" t="s">
         <v>8</v>
       </c>
@@ -7502,7 +7416,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A237" s="5" t="s">
         <v>8</v>
       </c>
@@ -7527,7 +7441,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A238" s="5" t="s">
         <v>8</v>
       </c>
@@ -7552,7 +7466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A239" s="4" t="s">
         <v>8</v>
       </c>
@@ -7560,9 +7474,11 @@
         <v>216</v>
       </c>
       <c r="C239" s="27">
+        <f>SUM(C235:C238)</f>
         <v>0</v>
       </c>
       <c r="D239" s="27">
+        <f>SUM(D235:D238)</f>
         <v>0</v>
       </c>
       <c r="E239" s="49" t="str">
@@ -7577,7 +7493,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A240" s="4" t="s">
         <v>8</v>
       </c>
@@ -7590,7 +7506,7 @@
       <c r="F240" s="50"/>
       <c r="G240" s="30"/>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A241" s="5" t="s">
         <v>8</v>
       </c>
@@ -7615,7 +7531,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A242" s="5" t="s">
         <v>8</v>
       </c>
@@ -7640,7 +7556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A243" s="5" t="s">
         <v>8</v>
       </c>
@@ -7665,7 +7581,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A244" s="5" t="s">
         <v>8</v>
       </c>
@@ -7690,7 +7606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A245" s="4" t="s">
         <v>8</v>
       </c>
@@ -7698,9 +7614,11 @@
         <v>217</v>
       </c>
       <c r="C245" s="27">
+        <f>SUM(C241:C244)</f>
         <v>0</v>
       </c>
       <c r="D245" s="27">
+        <f>SUM(D241:D244)</f>
         <v>0</v>
       </c>
       <c r="E245" s="49" t="str">
@@ -7715,7 +7633,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A246" s="4">
         <v>20</v>
       </c>
@@ -7728,7 +7646,7 @@
       <c r="F246" s="50"/>
       <c r="G246" s="30"/>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A247" s="5" t="s">
         <v>8</v>
       </c>
@@ -7743,7 +7661,7 @@
       <c r="F247" s="50"/>
       <c r="G247" s="29"/>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A248" s="5" t="s">
         <v>8</v>
       </c>
@@ -7768,7 +7686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A249" s="5" t="s">
         <v>8</v>
       </c>
@@ -7793,7 +7711,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A250" s="5" t="s">
         <v>8</v>
       </c>
@@ -7818,7 +7736,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A251" s="5"/>
       <c r="B251" s="5" t="s">
         <v>134</v>
@@ -7841,7 +7759,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A252" s="5"/>
       <c r="B252" s="5" t="s">
         <v>135</v>
@@ -7864,7 +7782,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A253" s="5"/>
       <c r="B253" s="5" t="s">
         <v>136</v>
@@ -7887,7 +7805,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A254" s="5"/>
       <c r="B254" s="5" t="s">
         <v>137</v>
@@ -7910,7 +7828,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A255" s="5"/>
       <c r="B255" s="5" t="s">
         <v>138</v>
@@ -7933,7 +7851,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A256" s="5"/>
       <c r="B256" s="5" t="s">
         <v>139</v>
@@ -7956,7 +7874,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A257" s="5"/>
       <c r="B257" s="5" t="s">
         <v>276</v>
@@ -7979,7 +7897,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A258" s="5"/>
       <c r="B258" s="5" t="s">
         <v>140</v>
@@ -8002,7 +7920,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A259" s="5" t="s">
         <v>8</v>
       </c>
@@ -8027,7 +7945,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A260" s="5" t="s">
         <v>8</v>
       </c>
@@ -8052,7 +7970,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A261" s="5" t="s">
         <v>8</v>
       </c>
@@ -8077,7 +7995,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A262" s="5" t="s">
         <v>8</v>
       </c>
@@ -8102,7 +8020,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A263" s="5"/>
       <c r="B263" s="5" t="s">
         <v>145</v>
@@ -8117,7 +8035,7 @@
       <c r="F263" s="50"/>
       <c r="G263" s="29"/>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A264" s="5"/>
       <c r="B264" s="5" t="s">
         <v>146</v>
@@ -8140,7 +8058,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A265" s="5"/>
       <c r="B265" s="5" t="s">
         <v>147</v>
@@ -8163,7 +8081,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A266" s="5"/>
       <c r="B266" s="5" t="s">
         <v>148</v>
@@ -8186,7 +8104,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A267" s="5"/>
       <c r="B267" s="5" t="s">
         <v>149</v>
@@ -8209,15 +8127,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A268" s="5"/>
       <c r="B268" s="4" t="s">
         <v>271</v>
       </c>
       <c r="C268" s="27">
+        <f>SUM(C247:C267)</f>
         <v>0</v>
       </c>
       <c r="D268" s="27">
+        <f>SUM(D247:D267)</f>
         <v>0</v>
       </c>
       <c r="E268" s="49" t="str">
@@ -8232,7 +8152,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A269" s="4">
         <v>21</v>
       </c>
@@ -8245,7 +8165,7 @@
       <c r="F269" s="50"/>
       <c r="G269" s="30"/>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A270" s="5" t="s">
         <v>8</v>
       </c>
@@ -8270,7 +8190,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A271" s="5" t="s">
         <v>8</v>
       </c>
@@ -8295,7 +8215,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A272" s="5" t="s">
         <v>8</v>
       </c>
@@ -8320,7 +8240,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A273" s="5" t="s">
         <v>8</v>
       </c>
@@ -8345,7 +8265,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A274" s="5" t="s">
         <v>8</v>
       </c>
@@ -8370,7 +8290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A275" s="5" t="s">
         <v>8</v>
       </c>
@@ -8395,7 +8315,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A276" s="5" t="s">
         <v>8</v>
       </c>
@@ -8420,7 +8340,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A277" s="5"/>
       <c r="B277" s="5" t="s">
         <v>158</v>
@@ -8443,7 +8363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A278" s="5" t="s">
         <v>8</v>
       </c>
@@ -8451,9 +8371,11 @@
         <v>218</v>
       </c>
       <c r="C278" s="27">
+        <f>SUM(C270:C277)</f>
         <v>0</v>
       </c>
       <c r="D278" s="27">
+        <f>SUM(D270:D277)</f>
         <v>0</v>
       </c>
       <c r="E278" s="49" t="str">
@@ -8468,7 +8390,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A279" s="4">
         <v>22</v>
       </c>
@@ -8481,7 +8403,7 @@
       <c r="F279" s="50"/>
       <c r="G279" s="30"/>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A280" s="5" t="s">
         <v>8</v>
       </c>
@@ -8506,7 +8428,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A281" s="5" t="s">
         <v>8</v>
       </c>
@@ -8531,7 +8453,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A282" s="5" t="s">
         <v>8</v>
       </c>
@@ -8556,7 +8478,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A283" s="5" t="s">
         <v>8</v>
       </c>
@@ -8581,7 +8503,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A284" s="5" t="s">
         <v>8</v>
       </c>
@@ -8606,7 +8528,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A285" s="4">
         <v>23</v>
       </c>
@@ -8619,7 +8541,7 @@
       <c r="F285" s="50"/>
       <c r="G285" s="30"/>
     </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A286" s="5" t="s">
         <v>8</v>
       </c>
@@ -8644,7 +8566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A287" s="5" t="s">
         <v>8</v>
       </c>
@@ -8669,7 +8591,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A288" s="10"/>
       <c r="B288" s="11" t="s">
         <v>96</v>
@@ -8692,7 +8614,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A289" s="5" t="s">
         <v>8</v>
       </c>
@@ -8717,7 +8639,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A290" s="5" t="s">
         <v>8</v>
       </c>
@@ -8742,7 +8664,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A291" s="4">
         <v>24</v>
       </c>
@@ -8755,7 +8677,7 @@
       <c r="F291" s="50"/>
       <c r="G291" s="30"/>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A292" s="5"/>
       <c r="B292" s="5" t="s">
         <v>162</v>
@@ -8778,7 +8700,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A293" s="5"/>
       <c r="B293" s="5" t="s">
         <v>95</v>
@@ -8801,7 +8723,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A294" s="5"/>
       <c r="B294" s="5" t="s">
         <v>96</v>
@@ -8824,7 +8746,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A295" s="5"/>
       <c r="B295" s="5" t="s">
         <v>97</v>
@@ -8847,7 +8769,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A296" s="5"/>
       <c r="B296" s="5" t="s">
         <v>160</v>
@@ -8870,7 +8792,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A297" s="4">
         <v>25</v>
       </c>
@@ -8883,7 +8805,7 @@
       <c r="F297" s="50"/>
       <c r="G297" s="30"/>
     </row>
-    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A298" s="5" t="s">
         <v>8</v>
       </c>
@@ -8908,7 +8830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A299" s="5" t="s">
         <v>8</v>
       </c>
@@ -8933,7 +8855,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A300" s="5" t="s">
         <v>8</v>
       </c>
@@ -8958,7 +8880,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A301" s="5" t="s">
         <v>8</v>
       </c>
@@ -8983,7 +8905,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A302" s="5" t="s">
         <v>8</v>
       </c>
@@ -9008,7 +8930,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="303" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A303" s="4">
         <v>26</v>
       </c>
@@ -9021,7 +8943,7 @@
       <c r="F303" s="50"/>
       <c r="G303" s="37"/>
     </row>
-    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A304" s="5"/>
       <c r="B304" s="5" t="s">
         <v>93</v>
@@ -9044,7 +8966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A305" s="5"/>
       <c r="B305" s="5" t="s">
         <v>95</v>
@@ -9067,7 +8989,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A306" s="5"/>
       <c r="B306" s="5" t="s">
         <v>96</v>
@@ -9090,7 +9012,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A307" s="5"/>
       <c r="B307" s="5" t="s">
         <v>97</v>
@@ -9113,7 +9035,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A308" s="5"/>
       <c r="B308" s="5" t="s">
         <v>160</v>
@@ -9136,7 +9058,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A309" s="4">
         <v>27</v>
       </c>
@@ -9149,7 +9071,7 @@
       <c r="F309" s="50"/>
       <c r="G309" s="37"/>
     </row>
-    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A310" s="5"/>
       <c r="B310" s="5" t="s">
         <v>93</v>
@@ -9172,7 +9094,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A311" s="5"/>
       <c r="B311" s="5" t="s">
         <v>95</v>
@@ -9195,7 +9117,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A312" s="5"/>
       <c r="B312" s="5" t="s">
         <v>96</v>
@@ -9218,7 +9140,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A313" s="5"/>
       <c r="B313" s="5" t="s">
         <v>97</v>
@@ -9241,7 +9163,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A314" s="5"/>
       <c r="B314" s="5" t="s">
         <v>160</v>
@@ -9264,7 +9186,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A315" s="4">
         <v>28</v>
       </c>
@@ -9277,7 +9199,7 @@
       <c r="F315" s="50"/>
       <c r="G315" s="37"/>
     </row>
-    <row r="316" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A316" s="5"/>
       <c r="B316" s="5" t="s">
         <v>93</v>
@@ -9300,7 +9222,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A317" s="5"/>
       <c r="B317" s="5" t="s">
         <v>95</v>
@@ -9323,7 +9245,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="318" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A318" s="5"/>
       <c r="B318" s="5" t="s">
         <v>96</v>
@@ -9346,7 +9268,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A319" s="5"/>
       <c r="B319" s="5" t="s">
         <v>97</v>
@@ -9369,7 +9291,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="320" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A320" s="5"/>
       <c r="B320" s="5" t="s">
         <v>160</v>
@@ -9392,7 +9314,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="321" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A321" s="4">
         <v>29</v>
       </c>
@@ -9409,7 +9331,7 @@
       <c r="F321" s="50"/>
       <c r="G321" s="30"/>
     </row>
-    <row r="322" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A322" s="4"/>
       <c r="B322" s="5" t="s">
         <v>93</v>
@@ -9432,7 +9354,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="323" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A323" s="5" t="s">
         <v>8</v>
       </c>
@@ -9457,7 +9379,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="324" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A324" s="5" t="s">
         <v>8</v>
       </c>
@@ -9482,7 +9404,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="325" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A325" s="5" t="s">
         <v>8</v>
       </c>
@@ -9507,7 +9429,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="326" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A326" s="5" t="s">
         <v>8</v>
       </c>
@@ -9532,7 +9454,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="327" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A327" s="5" t="s">
         <v>8</v>
       </c>
@@ -9557,7 +9479,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="328" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A328" s="5"/>
       <c r="B328" s="5" t="s">
         <v>168</v>
@@ -9580,7 +9502,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="329" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A329" s="4">
         <v>30</v>
       </c>
@@ -9597,7 +9519,7 @@
       <c r="F329" s="50"/>
       <c r="G329" s="29"/>
     </row>
-    <row r="330" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A330" s="5"/>
       <c r="B330" s="5" t="s">
         <v>225</v>
@@ -9620,7 +9542,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="331" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A331" s="5"/>
       <c r="B331" s="5" t="s">
         <v>226</v>
@@ -9643,7 +9565,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="332" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A332" s="5"/>
       <c r="B332" s="5" t="s">
         <v>227</v>
@@ -9666,15 +9588,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="333" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A333" s="5"/>
       <c r="B333" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C333" s="27">
+        <f>SUM(C330:C332)</f>
         <v>0</v>
       </c>
       <c r="D333" s="27">
+        <f>SUM(D330:D332)</f>
         <v>0</v>
       </c>
       <c r="E333" s="49" t="str">
@@ -9689,7 +9613,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="334" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A334" s="13" t="s">
         <v>263</v>
       </c>
@@ -9702,7 +9626,7 @@
       <c r="F334" s="50"/>
       <c r="G334" s="29"/>
     </row>
-    <row r="335" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A335" s="4">
         <v>31</v>
       </c>
@@ -9715,7 +9639,7 @@
       <c r="F335" s="50"/>
       <c r="G335" s="29"/>
     </row>
-    <row r="336" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A336" s="5"/>
       <c r="B336" s="21" t="s">
         <v>176</v>
@@ -9726,7 +9650,7 @@
       <c r="F336" s="50"/>
       <c r="G336" s="29"/>
     </row>
-    <row r="337" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A337" s="5"/>
       <c r="B337" s="22" t="s">
         <v>177</v>
@@ -9749,7 +9673,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="338" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A338" s="5"/>
       <c r="B338" s="22" t="s">
         <v>178</v>
@@ -9772,7 +9696,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="339" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A339" s="5"/>
       <c r="B339" s="52" t="s">
         <v>281</v>
@@ -9795,7 +9719,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="340" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A340" s="5"/>
       <c r="B340" s="22" t="s">
         <v>282</v>
@@ -9818,7 +9742,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="341" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A341" s="5"/>
       <c r="B341" s="22" t="s">
         <v>283</v>
@@ -9841,7 +9765,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="342" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A342" s="5"/>
       <c r="B342" s="22" t="s">
         <v>284</v>
@@ -9864,15 +9788,17 @@
         <v>107</v>
       </c>
     </row>
-    <row r="343" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A343" s="5"/>
       <c r="B343" s="22" t="s">
         <v>274</v>
       </c>
       <c r="C343" s="27">
+        <f>SUM(C337:C342)</f>
         <v>0</v>
       </c>
       <c r="D343" s="27">
+        <f>SUM(D337:D342)</f>
         <v>0</v>
       </c>
       <c r="E343" s="49" t="str">
@@ -9887,7 +9813,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="344" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A344" s="5"/>
       <c r="B344" s="21" t="s">
         <v>179</v>
@@ -9898,7 +9824,7 @@
       <c r="F344" s="50"/>
       <c r="G344" s="29"/>
     </row>
-    <row r="345" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A345" s="5"/>
       <c r="B345" s="22" t="s">
         <v>180</v>
@@ -9921,7 +9847,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="346" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A346" s="5"/>
       <c r="B346" s="22" t="s">
         <v>181</v>
@@ -9944,7 +9870,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="347" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A347" s="5"/>
       <c r="B347" s="22" t="s">
         <v>182</v>
@@ -9967,7 +9893,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="348" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A348" s="5"/>
       <c r="B348" s="22" t="s">
         <v>183</v>
@@ -9990,15 +9916,17 @@
         <v>107</v>
       </c>
     </row>
-    <row r="349" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A349" s="5"/>
       <c r="B349" s="22" t="s">
         <v>274</v>
       </c>
       <c r="C349" s="27">
+        <f>SUM(C345:C348)</f>
         <v>0</v>
       </c>
       <c r="D349" s="27">
+        <f>SUM(D345:D348)</f>
         <v>0</v>
       </c>
       <c r="E349" s="49" t="str">
@@ -10013,7 +9941,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="350" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A350" s="5"/>
       <c r="B350" s="21" t="s">
         <v>184</v>
@@ -10024,7 +9952,7 @@
       <c r="F350" s="50"/>
       <c r="G350" s="43"/>
     </row>
-    <row r="351" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A351" s="5"/>
       <c r="B351" s="22" t="s">
         <v>185</v>
@@ -10047,7 +9975,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="352" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A352" s="5"/>
       <c r="B352" s="22" t="s">
         <v>186</v>
@@ -10070,7 +9998,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="353" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A353" s="5"/>
       <c r="B353" s="22" t="s">
         <v>187</v>
@@ -10093,7 +10021,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="354" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A354" s="5"/>
       <c r="B354" s="22" t="s">
         <v>188</v>
@@ -10116,15 +10044,17 @@
         <v>107</v>
       </c>
     </row>
-    <row r="355" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A355" s="5"/>
       <c r="B355" s="21" t="s">
         <v>11</v>
       </c>
       <c r="C355" s="27">
+        <f>SUM(C351:C354)</f>
         <v>0</v>
       </c>
       <c r="D355" s="27">
+        <f>SUM(D351:D354)</f>
         <v>0</v>
       </c>
       <c r="E355" s="49" t="str">
@@ -10139,7 +10069,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="356" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A356" s="5"/>
       <c r="B356" s="21" t="s">
         <v>189</v>
@@ -10150,7 +10080,7 @@
       <c r="F356" s="50"/>
       <c r="G356" s="29"/>
     </row>
-    <row r="357" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A357" s="5"/>
       <c r="B357" s="22" t="s">
         <v>190</v>
@@ -10173,7 +10103,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="358" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A358" s="5"/>
       <c r="B358" s="22" t="s">
         <v>196</v>
@@ -10196,7 +10126,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="359" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A359" s="10"/>
       <c r="B359" s="11" t="s">
         <v>200</v>
@@ -10219,7 +10149,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="360" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A360" s="5"/>
       <c r="B360" s="22" t="s">
         <v>197</v>
@@ -10242,7 +10172,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="361" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A361" s="5"/>
       <c r="B361" s="22" t="s">
         <v>198</v>
@@ -10265,7 +10195,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="362" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A362" s="5"/>
       <c r="B362" s="22" t="s">
         <v>199</v>
@@ -10288,7 +10218,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="363" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A363" s="5"/>
       <c r="B363" s="22" t="s">
         <v>201</v>
@@ -10311,15 +10241,17 @@
         <v>107</v>
       </c>
     </row>
-    <row r="364" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A364" s="5"/>
       <c r="B364" s="21" t="s">
         <v>11</v>
       </c>
       <c r="C364" s="27">
+        <f>SUM(C357:C363)</f>
         <v>0</v>
       </c>
       <c r="D364" s="27">
+        <f>SUM(D357:D363)</f>
         <v>0</v>
       </c>
       <c r="E364" s="49" t="str">
@@ -10334,7 +10266,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="365" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A365" s="3" t="s">
         <v>228</v>
       </c>
@@ -10347,7 +10279,7 @@
       <c r="F365" s="50"/>
       <c r="G365" s="42"/>
     </row>
-    <row r="366" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A366" s="23">
         <v>32</v>
       </c>
@@ -10368,7 +10300,7 @@
       </c>
       <c r="G366" s="29"/>
     </row>
-    <row r="367" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A367" s="23"/>
       <c r="B367" s="22" t="s">
         <v>191</v>
@@ -10391,7 +10323,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="368" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A368" s="23"/>
       <c r="B368" s="22" t="s">
         <v>192</v>
@@ -10414,7 +10346,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="369" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A369" s="23"/>
       <c r="B369" s="22" t="s">
         <v>193</v>
@@ -10437,7 +10369,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="370" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A370" s="23"/>
       <c r="B370" s="22" t="s">
         <v>194</v>
@@ -10460,15 +10392,17 @@
         <v>107</v>
       </c>
     </row>
-    <row r="371" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A371" s="23"/>
       <c r="B371" s="21" t="s">
         <v>11</v>
       </c>
       <c r="C371" s="27">
+        <f>SUM(C367:C370)</f>
         <v>0</v>
       </c>
       <c r="D371" s="27">
+        <f>SUM(D367:D370)</f>
         <v>0</v>
       </c>
       <c r="E371" s="49" t="str">
@@ -10483,7 +10417,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="372" spans="1:7" s="60" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:7" s="60" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A372" s="53" t="s">
         <v>260</v>
       </c>
@@ -10496,7 +10430,7 @@
       <c r="F372" s="58"/>
       <c r="G372" s="59"/>
     </row>
-    <row r="373" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A373" s="61">
         <v>33</v>
       </c>
@@ -10509,7 +10443,7 @@
       <c r="F373" s="58"/>
       <c r="G373" s="59"/>
     </row>
-    <row r="374" spans="1:7" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:7" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A374" s="64" t="s">
         <v>234</v>
       </c>
@@ -10522,7 +10456,7 @@
       <c r="F374" s="58"/>
       <c r="G374" s="59"/>
     </row>
-    <row r="375" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A375" s="64"/>
       <c r="B375" s="64" t="s">
         <v>236</v>
@@ -10545,7 +10479,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="376" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A376" s="64"/>
       <c r="B376" s="64" t="s">
         <v>237</v>
@@ -10568,7 +10502,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="377" spans="1:7" s="60" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:7" s="60" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A377" s="64"/>
       <c r="B377" s="64" t="s">
         <v>238</v>
@@ -10591,7 +10525,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="378" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A378" s="64"/>
       <c r="B378" s="64" t="s">
         <v>239</v>
@@ -10614,7 +10548,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="379" spans="1:7" s="60" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:7" s="60" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A379" s="64"/>
       <c r="B379" s="65" t="s">
         <v>240</v>
@@ -10637,7 +10571,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="380" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A380" s="64"/>
       <c r="B380" s="65" t="s">
         <v>241</v>
@@ -10660,7 +10594,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="381" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A381" s="64"/>
       <c r="B381" s="65" t="s">
         <v>242</v>
@@ -10683,7 +10617,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="382" spans="1:7" s="60" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:7" s="60" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A382" s="64"/>
       <c r="B382" s="65" t="s">
         <v>243</v>
@@ -10706,7 +10640,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="383" spans="1:7" s="60" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:7" s="60" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A383" s="64"/>
       <c r="B383" s="65" t="s">
         <v>244</v>
@@ -10729,7 +10663,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="384" spans="1:7" s="60" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:7" s="60" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A384" s="64" t="s">
         <v>234</v>
       </c>
@@ -10742,7 +10676,7 @@
       <c r="F384" s="58"/>
       <c r="G384" s="71"/>
     </row>
-    <row r="385" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A385" s="64"/>
       <c r="B385" s="65" t="s">
         <v>246</v>
@@ -10765,7 +10699,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="386" spans="1:7" s="60" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:7" s="60" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A386" s="64"/>
       <c r="B386" s="65" t="s">
         <v>242</v>
@@ -10788,7 +10722,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="387" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A387" s="64"/>
       <c r="B387" s="65" t="s">
         <v>244</v>
@@ -10811,7 +10745,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="388" spans="1:7" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:7" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A388" s="64" t="s">
         <v>234</v>
       </c>
@@ -10826,7 +10760,7 @@
       <c r="F388" s="58"/>
       <c r="G388" s="72"/>
     </row>
-    <row r="389" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A389" s="64"/>
       <c r="B389" s="64" t="s">
         <v>248</v>
@@ -10849,7 +10783,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="390" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A390" s="64"/>
       <c r="B390" s="64" t="s">
         <v>249</v>
@@ -10872,7 +10806,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="391" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A391" s="64"/>
       <c r="B391" s="64" t="s">
         <v>250</v>
@@ -10895,7 +10829,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="392" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A392" s="64"/>
       <c r="B392" s="64" t="s">
         <v>237</v>
@@ -10918,7 +10852,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="393" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A393" s="64"/>
       <c r="B393" s="64" t="s">
         <v>251</v>
@@ -10941,7 +10875,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="394" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A394" s="64"/>
       <c r="B394" s="64" t="s">
         <v>249</v>
@@ -10964,7 +10898,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="395" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A395" s="64"/>
       <c r="B395" s="64" t="s">
         <v>250</v>
@@ -10987,7 +10921,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="396" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A396" s="64"/>
       <c r="B396" s="64" t="s">
         <v>239</v>
@@ -11010,7 +10944,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="397" spans="1:7" s="60" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:7" s="60" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A397" s="64"/>
       <c r="B397" s="65" t="s">
         <v>254</v>
@@ -11033,7 +10967,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="398" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A398" s="64"/>
       <c r="B398" s="65" t="s">
         <v>255</v>
@@ -11056,7 +10990,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="399" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A399" s="64"/>
       <c r="B399" s="65" t="s">
         <v>256</v>
@@ -11079,7 +11013,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="400" spans="1:7" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:7" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A400" s="64"/>
       <c r="B400" s="65" t="s">
         <v>242</v>
@@ -11102,7 +11036,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="401" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A401" s="64"/>
       <c r="B401" s="65" t="s">
         <v>244</v>
@@ -11125,7 +11059,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="402" spans="1:7" s="60" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:7" s="60" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A402" s="64" t="s">
         <v>234</v>
       </c>
@@ -11138,7 +11072,7 @@
       <c r="F402" s="58"/>
       <c r="G402" s="72"/>
     </row>
-    <row r="403" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A403" s="64"/>
       <c r="B403" s="64" t="s">
         <v>258</v>
@@ -11161,7 +11095,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="404" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A404" s="64"/>
       <c r="B404" s="64" t="s">
         <v>259</v>
@@ -11184,7 +11118,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="405" spans="1:7" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:7" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A405" s="64"/>
       <c r="B405" s="65" t="s">
         <v>265</v>
@@ -11207,7 +11141,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="406" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A406" s="64"/>
       <c r="B406" s="65" t="s">
         <v>242</v>
@@ -11230,7 +11164,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="407" spans="1:7" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:7" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A407" s="64"/>
       <c r="B407" s="65" t="s">
         <v>244</v>
@@ -11253,7 +11187,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="408" spans="1:7" s="60" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:7" s="60" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A408" s="53" t="s">
         <v>285</v>
       </c>
@@ -11266,7 +11200,7 @@
       <c r="F408" s="58"/>
       <c r="G408" s="59"/>
     </row>
-    <row r="409" spans="1:7" s="60" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:7" s="60" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A409" s="61">
         <v>34</v>
       </c>
@@ -11279,7 +11213,7 @@
       <c r="F409" s="58"/>
       <c r="G409" s="59"/>
     </row>
-    <row r="410" spans="1:7" s="60" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:7" s="60" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A410" s="64"/>
       <c r="B410" s="76" t="s">
         <v>288</v>
@@ -11302,7 +11236,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="411" spans="1:7" s="60" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:7" s="60" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A411" s="64"/>
       <c r="B411" s="76" t="s">
         <v>289</v>
@@ -11325,7 +11259,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="412" spans="1:7" s="60" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:7" s="60" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A412" s="64"/>
       <c r="B412" s="76" t="s">
         <v>290</v>
@@ -11348,7 +11282,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="413" spans="1:7" s="60" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:7" s="60" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A413" s="64"/>
       <c r="B413" s="76" t="s">
         <v>291</v>
@@ -11371,32 +11305,32 @@
         <v>107</v>
       </c>
     </row>
-    <row r="414" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A414" s="77"/>
       <c r="B414" s="78" t="s">
         <v>11</v>
       </c>
       <c r="C414" s="79">
-        <f t="shared" ref="C414:D414" si="18">SUM(C409:C413)</f>
-        <v>0</v>
-      </c>
-      <c r="D414" s="80">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="E414" s="81" t="str">
+        <f>SUM(C410:C413)</f>
+        <v>0</v>
+      </c>
+      <c r="D414" s="79">
+        <f>SUM(D410:D413)</f>
+        <v>0</v>
+      </c>
+      <c r="E414" s="80" t="str">
         <f>IF(C414=D414,"TETAP", IF(C414&gt;D414, "TURUN","NAIK"))</f>
         <v>TETAP</v>
       </c>
-      <c r="F414" s="82" t="e">
+      <c r="F414" s="81" t="e">
         <f>SUM(D414-C414)/C414*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G414" s="83" t="s">
+      <c r="G414" s="82" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="415" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A415" s="46"/>
       <c r="B415" s="46"/>
       <c r="C415" s="46"/>
@@ -11405,7 +11339,7 @@
       <c r="F415" s="87"/>
       <c r="G415" s="87"/>
     </row>
-    <row r="416" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A416" s="46"/>
       <c r="B416" s="46"/>
       <c r="C416" s="46"/>
@@ -11414,30 +11348,30 @@
       <c r="F416" s="46"/>
       <c r="G416" s="46"/>
     </row>
-    <row r="417" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A417" s="46"/>
       <c r="B417" s="46"/>
       <c r="C417" s="46"/>
       <c r="D417" s="46"/>
-      <c r="E417" s="97" t="s">
+      <c r="E417" s="86" t="s">
         <v>293</v>
       </c>
-      <c r="F417" s="97"/>
+      <c r="F417" s="86"/>
       <c r="G417" s="46"/>
     </row>
-    <row r="418" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A418" s="46"/>
       <c r="B418" s="46"/>
       <c r="C418" s="46"/>
       <c r="D418" s="46"/>
-      <c r="E418" s="97"/>
-      <c r="F418" s="97"/>
+      <c r="E418" s="86"/>
+      <c r="F418" s="86"/>
       <c r="G418" s="46"/>
     </row>
-    <row r="419" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A419" s="46"/>
       <c r="B419" s="46"/>
-      <c r="C419" s="86"/>
+      <c r="C419" s="85"/>
       <c r="D419" s="46"/>
       <c r="E419" s="87" t="s">
         <v>294</v>
@@ -11445,65 +11379,65 @@
       <c r="F419" s="87"/>
       <c r="G419" s="46"/>
     </row>
-    <row r="420" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A420" s="46"/>
       <c r="B420" s="46"/>
-      <c r="C420" s="86"/>
+      <c r="C420" s="85"/>
       <c r="D420" s="46"/>
       <c r="E420" s="46"/>
       <c r="F420" s="46"/>
       <c r="G420" s="46"/>
     </row>
-    <row r="421" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A421" s="46"/>
       <c r="B421" s="46"/>
-      <c r="C421" s="86"/>
+      <c r="C421" s="85"/>
       <c r="D421" s="46"/>
       <c r="E421" s="46"/>
       <c r="F421" s="46"/>
       <c r="G421" s="46"/>
     </row>
-    <row r="422" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A422" s="46"/>
       <c r="B422" s="46"/>
-      <c r="C422" s="86"/>
+      <c r="C422" s="85"/>
       <c r="D422" s="46"/>
       <c r="E422" s="46"/>
       <c r="F422" s="46"/>
       <c r="G422" s="46"/>
     </row>
-    <row r="423" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A423" s="46"/>
       <c r="B423" s="46"/>
-      <c r="C423" s="86"/>
+      <c r="C423" s="85"/>
       <c r="D423" s="46"/>
       <c r="E423" s="46"/>
       <c r="F423" s="46"/>
       <c r="G423" s="46"/>
     </row>
-    <row r="424" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A424" s="46"/>
       <c r="B424" s="46"/>
-      <c r="C424" s="86"/>
+      <c r="C424" s="85"/>
       <c r="D424" s="46"/>
-      <c r="E424" s="97" t="s">
+      <c r="E424" s="86" t="s">
         <v>295</v>
       </c>
-      <c r="F424" s="97"/>
+      <c r="F424" s="86"/>
       <c r="G424" s="46"/>
     </row>
-    <row r="425" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A425" s="46"/>
       <c r="B425" s="46"/>
-      <c r="C425" s="86"/>
+      <c r="C425" s="85"/>
       <c r="D425" s="46"/>
-      <c r="E425" s="97" t="s">
+      <c r="E425" s="86" t="s">
         <v>296</v>
       </c>
-      <c r="F425" s="97"/>
+      <c r="F425" s="86"/>
       <c r="G425" s="46"/>
     </row>
-    <row r="426" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A426" s="46"/>
       <c r="B426" s="46"/>
       <c r="C426" s="46"/>
@@ -11512,7 +11446,7 @@
       <c r="F426" s="46"/>
       <c r="G426" s="46"/>
     </row>
-    <row r="427" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A427" s="46"/>
       <c r="B427" s="46"/>
       <c r="C427" s="46"/>
@@ -11521,7 +11455,7 @@
       <c r="F427" s="46"/>
       <c r="G427" s="46"/>
     </row>
-    <row r="428" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A428" s="46"/>
       <c r="B428" s="46"/>
       <c r="C428" s="46"/>
@@ -11530,7 +11464,7 @@
       <c r="F428" s="46"/>
       <c r="G428" s="46"/>
     </row>
-    <row r="429" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A429" s="46"/>
       <c r="B429" s="46"/>
       <c r="C429" s="46"/>
@@ -11539,7 +11473,7 @@
       <c r="F429" s="46"/>
       <c r="G429" s="46"/>
     </row>
-    <row r="430" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A430" s="46"/>
       <c r="B430" s="46"/>
       <c r="C430" s="46"/>
@@ -11548,7 +11482,7 @@
       <c r="F430" s="46"/>
       <c r="G430" s="46"/>
     </row>
-    <row r="431" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A431" s="46"/>
       <c r="B431" s="46"/>
       <c r="C431" s="46"/>
@@ -11557,7 +11491,7 @@
       <c r="F431" s="46"/>
       <c r="G431" s="46"/>
     </row>
-    <row r="432" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A432" s="46"/>
       <c r="B432" s="46"/>
       <c r="C432" s="46"/>
@@ -11566,7 +11500,7 @@
       <c r="F432" s="46"/>
       <c r="G432" s="46"/>
     </row>
-    <row r="433" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A433" s="46"/>
       <c r="B433" s="46"/>
       <c r="C433" s="46"/>
@@ -11575,7 +11509,7 @@
       <c r="F433" s="46"/>
       <c r="G433" s="46"/>
     </row>
-    <row r="434" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A434" s="46"/>
       <c r="B434" s="46"/>
       <c r="C434" s="46"/>
@@ -11584,7 +11518,7 @@
       <c r="F434" s="46"/>
       <c r="G434" s="46"/>
     </row>
-    <row r="435" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A435" s="46"/>
       <c r="B435" s="46"/>
       <c r="C435" s="46"/>
@@ -11593,7 +11527,7 @@
       <c r="F435" s="46"/>
       <c r="G435" s="46"/>
     </row>
-    <row r="436" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A436" s="46"/>
       <c r="B436" s="46"/>
       <c r="C436" s="46"/>
@@ -11602,7 +11536,7 @@
       <c r="F436" s="46"/>
       <c r="G436" s="46"/>
     </row>
-    <row r="437" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A437" s="46"/>
       <c r="B437" s="46"/>
       <c r="C437" s="46"/>
@@ -11611,7 +11545,7 @@
       <c r="F437" s="46"/>
       <c r="G437" s="46"/>
     </row>
-    <row r="438" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A438" s="46"/>
       <c r="B438" s="46"/>
       <c r="C438" s="46"/>
@@ -11620,7 +11554,7 @@
       <c r="F438" s="46"/>
       <c r="G438" s="46"/>
     </row>
-    <row r="439" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A439" s="46"/>
       <c r="B439" s="46"/>
       <c r="C439" s="46"/>
@@ -11629,7 +11563,7 @@
       <c r="F439" s="46"/>
       <c r="G439" s="46"/>
     </row>
-    <row r="440" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A440" s="46"/>
       <c r="B440" s="46"/>
       <c r="C440" s="46"/>
@@ -11638,7 +11572,7 @@
       <c r="F440" s="46"/>
       <c r="G440" s="46"/>
     </row>
-    <row r="441" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A441" s="46"/>
       <c r="B441" s="46"/>
       <c r="C441" s="46"/>
@@ -11647,7 +11581,7 @@
       <c r="F441" s="46"/>
       <c r="G441" s="46"/>
     </row>
-    <row r="442" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A442" s="46"/>
       <c r="B442" s="46"/>
       <c r="C442" s="46"/>
@@ -11656,7 +11590,7 @@
       <c r="F442" s="46"/>
       <c r="G442" s="46"/>
     </row>
-    <row r="443" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A443" s="46"/>
       <c r="B443" s="46"/>
       <c r="C443" s="46"/>
@@ -11665,7 +11599,7 @@
       <c r="F443" s="46"/>
       <c r="G443" s="46"/>
     </row>
-    <row r="444" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A444" s="46"/>
       <c r="B444" s="46"/>
       <c r="C444" s="46"/>
@@ -11674,7 +11608,7 @@
       <c r="F444" s="46"/>
       <c r="G444" s="46"/>
     </row>
-    <row r="445" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A445" s="46"/>
       <c r="B445" s="46"/>
       <c r="C445" s="46"/>
@@ -11683,7 +11617,7 @@
       <c r="F445" s="46"/>
       <c r="G445" s="46"/>
     </row>
-    <row r="446" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A446" s="46"/>
       <c r="B446" s="46"/>
       <c r="C446" s="46"/>
@@ -11692,7 +11626,7 @@
       <c r="F446" s="46"/>
       <c r="G446" s="46"/>
     </row>
-    <row r="447" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A447" s="46"/>
       <c r="B447" s="46"/>
       <c r="C447" s="46"/>
@@ -11701,7 +11635,7 @@
       <c r="F447" s="46"/>
       <c r="G447" s="46"/>
     </row>
-    <row r="448" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A448" s="46"/>
       <c r="B448" s="46"/>
       <c r="C448" s="46"/>
@@ -11710,7 +11644,7 @@
       <c r="F448" s="46"/>
       <c r="G448" s="46"/>
     </row>
-    <row r="449" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A449" s="46"/>
       <c r="B449" s="46"/>
       <c r="C449" s="46"/>
@@ -11719,7 +11653,7 @@
       <c r="F449" s="46"/>
       <c r="G449" s="46"/>
     </row>
-    <row r="450" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A450" s="46"/>
       <c r="B450" s="46"/>
       <c r="C450" s="46"/>
@@ -11728,7 +11662,7 @@
       <c r="F450" s="46"/>
       <c r="G450" s="46"/>
     </row>
-    <row r="451" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A451" s="46"/>
       <c r="B451" s="46"/>
       <c r="C451" s="46"/>
@@ -11737,7 +11671,7 @@
       <c r="F451" s="46"/>
       <c r="G451" s="46"/>
     </row>
-    <row r="452" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A452" s="46"/>
       <c r="B452" s="46"/>
       <c r="C452" s="46"/>
@@ -11746,7 +11680,7 @@
       <c r="F452" s="46"/>
       <c r="G452" s="46"/>
     </row>
-    <row r="453" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A453" s="46"/>
       <c r="B453" s="46"/>
       <c r="C453" s="46"/>
@@ -11755,7 +11689,7 @@
       <c r="F453" s="46"/>
       <c r="G453" s="46"/>
     </row>
-    <row r="454" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A454" s="46"/>
       <c r="B454" s="46"/>
       <c r="C454" s="46"/>
@@ -11764,7 +11698,7 @@
       <c r="F454" s="46"/>
       <c r="G454" s="46"/>
     </row>
-    <row r="455" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A455" s="46"/>
       <c r="B455" s="46"/>
       <c r="C455" s="46"/>
@@ -11773,7 +11707,7 @@
       <c r="F455" s="46"/>
       <c r="G455" s="46"/>
     </row>
-    <row r="456" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A456" s="46"/>
       <c r="B456" s="46"/>
       <c r="C456" s="46"/>
@@ -11782,7 +11716,7 @@
       <c r="F456" s="46"/>
       <c r="G456" s="46"/>
     </row>
-    <row r="457" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A457" s="46"/>
       <c r="B457" s="46"/>
       <c r="C457" s="46"/>
@@ -11791,7 +11725,7 @@
       <c r="F457" s="46"/>
       <c r="G457" s="46"/>
     </row>
-    <row r="458" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A458" s="46"/>
       <c r="B458" s="46"/>
       <c r="C458" s="46"/>
@@ -11800,7 +11734,7 @@
       <c r="F458" s="46"/>
       <c r="G458" s="46"/>
     </row>
-    <row r="459" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A459" s="46"/>
       <c r="B459" s="46"/>
       <c r="C459" s="46"/>
@@ -11809,7 +11743,7 @@
       <c r="F459" s="46"/>
       <c r="G459" s="46"/>
     </row>
-    <row r="460" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A460" s="46"/>
       <c r="B460" s="46"/>
       <c r="C460" s="46"/>
@@ -11818,7 +11752,7 @@
       <c r="F460" s="46"/>
       <c r="G460" s="46"/>
     </row>
-    <row r="461" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A461" s="46"/>
       <c r="B461" s="46"/>
       <c r="C461" s="46"/>
@@ -11827,7 +11761,7 @@
       <c r="F461" s="46"/>
       <c r="G461" s="46"/>
     </row>
-    <row r="462" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A462" s="46"/>
       <c r="B462" s="46"/>
       <c r="C462" s="46"/>
@@ -11836,7 +11770,7 @@
       <c r="F462" s="46"/>
       <c r="G462" s="46"/>
     </row>
-    <row r="463" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A463" s="46"/>
       <c r="B463" s="46"/>
       <c r="C463" s="46"/>
@@ -11845,7 +11779,7 @@
       <c r="F463" s="46"/>
       <c r="G463" s="46"/>
     </row>
-    <row r="464" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A464" s="46"/>
       <c r="B464" s="46"/>
       <c r="C464" s="46"/>
@@ -11854,7 +11788,7 @@
       <c r="F464" s="46"/>
       <c r="G464" s="46"/>
     </row>
-    <row r="465" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A465" s="46"/>
       <c r="B465" s="46"/>
       <c r="C465" s="46"/>
@@ -11863,7 +11797,7 @@
       <c r="F465" s="46"/>
       <c r="G465" s="46"/>
     </row>
-    <row r="466" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A466" s="46"/>
       <c r="B466" s="46"/>
       <c r="C466" s="46"/>
@@ -11872,22 +11806,17 @@
       <c r="F466" s="46"/>
       <c r="G466" s="46"/>
     </row>
-    <row r="469" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D469" s="48"/>
     </row>
-    <row r="470" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D470" s="48"/>
     </row>
-    <row r="471" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D471" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="E418:F418"/>
-    <mergeCell ref="E419:F419"/>
-    <mergeCell ref="E424:F424"/>
-    <mergeCell ref="E425:F425"/>
-    <mergeCell ref="E417:F417"/>
     <mergeCell ref="E415:G415"/>
     <mergeCell ref="A7:G7"/>
     <mergeCell ref="A1:B1"/>
@@ -11901,6 +11830,11 @@
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E418:F418"/>
+    <mergeCell ref="E419:F419"/>
+    <mergeCell ref="E424:F424"/>
+    <mergeCell ref="E425:F425"/>
+    <mergeCell ref="E417:F417"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.31496062992125984" top="0.23622047244094491" bottom="0.23622047244094491" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Fix bug new report
</commit_message>
<xml_diff>
--- a/public/template/excel/format_laporan_operasi_2021.xlsx
+++ b/public/template/excel/format_laporan_operasi_2021.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajoris\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\korlantas\public\template\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -884,16 +884,10 @@
     <t>Pelabuhan</t>
   </si>
   <si>
-    <t>Jakarta, 13 April 2021</t>
-  </si>
-  <si>
     <t>KAPOSKO</t>
   </si>
   <si>
     <t>NAMA XXXX</t>
-  </si>
-  <si>
-    <t>AKP NRP 83099999</t>
   </si>
   <si>
     <r>
@@ -957,6 +951,12 @@
   </si>
   <si>
     <t>a. Motor</t>
+  </si>
+  <si>
+    <t>AKP NRP 000000000</t>
+  </si>
+  <si>
+    <t>Jakarta, 01 Januari 2021</t>
   </si>
 </sst>
 </file>
@@ -2009,8 +2009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A406" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="178" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B427" sqref="B427"/>
+    <sheetView tabSelected="1" topLeftCell="A398" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="178" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="E417" sqref="E417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2070,7 +2070,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="39" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
@@ -2080,7 +2080,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="38" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C7" s="49"/>
       <c r="D7" s="49"/>
@@ -2190,7 +2190,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C14" s="50">
         <v>0</v>
@@ -8041,7 +8041,7 @@
     <row r="268" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A268" s="14"/>
       <c r="B268" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C268" s="50">
         <f>SUM(C247:C267)</f>
@@ -8457,7 +8457,7 @@
         <v>8</v>
       </c>
       <c r="B286" s="14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C286" s="50">
         <v>0</v>
@@ -9102,7 +9102,7 @@
         <v>28</v>
       </c>
       <c r="B315" s="7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C315" s="52"/>
       <c r="D315" s="64"/>
@@ -9702,7 +9702,7 @@
     <row r="343" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A343" s="14"/>
       <c r="B343" s="26" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C343" s="50">
         <f>SUM(C337:C342)</f>
@@ -9830,7 +9830,7 @@
     <row r="349" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A349" s="14"/>
       <c r="B349" s="26" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C349" s="50">
         <f>SUM(C345:C348)</f>
@@ -11233,10 +11233,10 @@
     </row>
     <row r="415" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A415" s="79" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B415" s="25" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C415" s="84"/>
       <c r="D415" s="65"/>
@@ -11247,7 +11247,7 @@
     <row r="416" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A416" s="37"/>
       <c r="B416" s="26" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C416" s="84">
         <v>0</v>
@@ -11256,6 +11256,7 @@
         <v>0</v>
       </c>
       <c r="E416" s="15">
+        <f>D416-C416</f>
         <v>0</v>
       </c>
       <c r="F416" s="81" t="e">
@@ -11278,6 +11279,7 @@
         <v>0</v>
       </c>
       <c r="E417" s="15">
+        <f t="shared" ref="E417:E421" si="46">D417-C417</f>
         <v>0</v>
       </c>
       <c r="F417" s="81" t="e">
@@ -11300,6 +11302,7 @@
         <v>0</v>
       </c>
       <c r="E418" s="15">
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="F418" s="81" t="e">
@@ -11322,6 +11325,7 @@
         <v>0</v>
       </c>
       <c r="E419" s="15">
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="F419" s="81" t="e">
@@ -11344,6 +11348,7 @@
         <v>0</v>
       </c>
       <c r="E420" s="15">
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="F420" s="81" t="e">
@@ -11367,8 +11372,8 @@
         <f>SUM(D416:D420)</f>
         <v>0</v>
       </c>
-      <c r="E421" s="83">
-        <f>SUM(E416:E420)</f>
+      <c r="E421" s="15">
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="F421" s="81" t="e">
@@ -11394,7 +11399,7 @@
       <c r="C423" s="62"/>
       <c r="D423" s="43"/>
       <c r="E423" s="94" t="s">
-        <v>284</v>
+        <v>297</v>
       </c>
       <c r="F423" s="94"/>
       <c r="G423" s="43"/>
@@ -11414,7 +11419,7 @@
       <c r="C425" s="62"/>
       <c r="D425" s="43"/>
       <c r="E425" s="95" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F425" s="95"/>
       <c r="G425" s="43"/>
@@ -11461,7 +11466,7 @@
       <c r="C430" s="62"/>
       <c r="D430" s="43"/>
       <c r="E430" s="94" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F430" s="94"/>
       <c r="G430" s="43"/>
@@ -11472,7 +11477,7 @@
       <c r="C431" s="62"/>
       <c r="D431" s="43"/>
       <c r="E431" s="94" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="F431" s="94"/>
       <c r="G431" s="43"/>

</xml_diff>